<commit_message>
changing I1 to rerun spline
</commit_message>
<xml_diff>
--- a/data/Charlie1124/case3/data-case3.xlsx
+++ b/data/Charlie1124/case3/data-case3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caesa/Desktop/CoCo/data/Charlie1124/case3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599A268E-DB33-AA43-8F72-7B2713E886D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09039D7-AEE5-F14E-AB6F-40310176815E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="720" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{5D9C6509-A9B6-B44E-9EE3-0A45CAFD3315}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="17720" activeTab="1" xr2:uid="{5D9C6509-A9B6-B44E-9EE3-0A45CAFD3315}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -69,36 +69,6 @@
   </si>
   <si>
     <t>Company Name</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>CET-1 ratio (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>phase-in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>LYG</t>
@@ -143,6 +113,114 @@
     <t>2023Q4</t>
   </si>
   <si>
+    <t>CET-1 ratio (phase-in)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>2013Q1</t>
+  </si>
+  <si>
+    <t>Pro forma, post-dividend</t>
+  </si>
+  <si>
+    <t>2013Q2</t>
+  </si>
+  <si>
+    <t>2013Q3</t>
+  </si>
+  <si>
+    <t>2013Q4</t>
+  </si>
+  <si>
+    <t>2014Q1</t>
+  </si>
+  <si>
+    <t>2014Q2</t>
+  </si>
+  <si>
+    <t>2014Q3</t>
+  </si>
+  <si>
+    <t>2014Q4</t>
+  </si>
+  <si>
+    <t>2015Q1</t>
+  </si>
+  <si>
+    <t>2015Q2</t>
+  </si>
+  <si>
+    <t>2015Q3</t>
+  </si>
+  <si>
+    <t>2015Q4</t>
+  </si>
+  <si>
+    <t>2016Q1</t>
+  </si>
+  <si>
+    <t>2016Q2</t>
+  </si>
+  <si>
+    <t>2016Q3</t>
+  </si>
+  <si>
+    <t>2016Q4</t>
+  </si>
+  <si>
+    <t>2017Q1</t>
+  </si>
+  <si>
+    <t>2017Q2</t>
+  </si>
+  <si>
+    <t>2017Q3</t>
+  </si>
+  <si>
+    <t>2017Q4</t>
+  </si>
+  <si>
+    <t>2018Q1</t>
+  </si>
+  <si>
+    <t>Implied from prev quarter</t>
+  </si>
+  <si>
+    <t>2018Q2</t>
+  </si>
+  <si>
+    <t>2018Q3</t>
+  </si>
+  <si>
+    <t>2018Q4</t>
+  </si>
+  <si>
+    <t>2019Q1</t>
+  </si>
+  <si>
+    <t>2019Q2</t>
+  </si>
+  <si>
+    <t>2019Q3</t>
+  </si>
+  <si>
+    <t>2019Q4</t>
+  </si>
+  <si>
+    <t>2020Q1</t>
+  </si>
+  <si>
+    <t>2020Q2</t>
+  </si>
+  <si>
+    <t>2020Q3</t>
+  </si>
+  <si>
+    <t>2020Q4</t>
+  </si>
+  <si>
     <t>2024Q1</t>
   </si>
 </sst>
@@ -153,7 +231,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00##_);[Red]\(#,##0.00##\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,13 +246,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -219,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -19429,15 +19500,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD21945-F66C-D342-B83B-FDECAD2EEF51}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -19448,188 +19519,645 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D10" s="4">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="4">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4">
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34">
         <v>16.7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4">
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="D36">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="D37">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="D38">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="D39">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43">
         <v>14.2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="4">
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="D44">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="D45">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="4">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="4">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="4">
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="D46">
         <v>13.7</v>
       </c>
     </row>

</xml_diff>